<commit_message>
Despues de mostrar avances a la instructora
</commit_message>
<xml_diff>
--- a/public/formatos/GTH_F_060__FORMATO_LEGALIZACION_DE_HORAS_EXTRAS_RECARGOS_NOCTURNOS_DOMINICALES.xlsx
+++ b/public/formatos/GTH_F_060__FORMATO_LEGALIZACION_DE_HORAS_EXTRAS_RECARGOS_NOCTURNOS_DOMINICALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\she\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2803950B-B105-4613-8B6B-73C98905424E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C07581-6174-469F-A347-1110A3EEB892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,6 +280,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+  </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1240,7 +1244,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1419,6 +1423,177 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="49" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1506,151 +1681,43 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1659,38 +1726,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2144,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3249,370 +3286,370 @@
   <sheetData>
     <row r="1" spans="2:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="65"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="67"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="124"/>
     </row>
     <row r="3" spans="2:26" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="70"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="127"/>
     </row>
     <row r="4" spans="2:26" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="78" t="s">
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="140"/>
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
+      <c r="W4" s="140"/>
+      <c r="X4" s="135" t="s">
         <v>63</v>
       </c>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="79"/>
+      <c r="Y4" s="135"/>
+      <c r="Z4" s="136"/>
     </row>
     <row r="5" spans="2:26" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="80" t="s">
+      <c r="B5" s="141"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="142"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="142"/>
+      <c r="Q5" s="142"/>
+      <c r="R5" s="142"/>
+      <c r="S5" s="142"/>
+      <c r="T5" s="142"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="142"/>
+      <c r="W5" s="142"/>
+      <c r="X5" s="137" t="s">
         <v>62</v>
       </c>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="81"/>
+      <c r="Y5" s="137"/>
+      <c r="Z5" s="138"/>
     </row>
     <row r="6" spans="2:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="74" t="s">
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="71" t="s">
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="133"/>
+      <c r="Q6" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="72"/>
-      <c r="V6" s="72"/>
-      <c r="W6" s="72"/>
-      <c r="X6" s="72"/>
-      <c r="Y6" s="72"/>
-      <c r="Z6" s="73"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="129"/>
+      <c r="U6" s="129"/>
+      <c r="V6" s="129"/>
+      <c r="W6" s="129"/>
+      <c r="X6" s="129"/>
+      <c r="Y6" s="129"/>
+      <c r="Z6" s="130"/>
     </row>
     <row r="7" spans="2:26" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="86"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="91"/>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="92"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="144"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="143"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="144"/>
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="148"/>
+      <c r="S7" s="148"/>
+      <c r="T7" s="148"/>
+      <c r="U7" s="148"/>
+      <c r="V7" s="148"/>
+      <c r="W7" s="148"/>
+      <c r="X7" s="148"/>
+      <c r="Y7" s="148"/>
+      <c r="Z7" s="149"/>
     </row>
     <row r="8" spans="2:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93" t="s">
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93" t="s">
+      <c r="P8" s="107"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="U8" s="93"/>
-      <c r="V8" s="93"/>
-      <c r="W8" s="93"/>
-      <c r="X8" s="93"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="93"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="107"/>
+      <c r="Y8" s="107"/>
+      <c r="Z8" s="107"/>
     </row>
     <row r="9" spans="2:26" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="165"/>
+      <c r="P9" s="165"/>
+      <c r="Q9" s="165"/>
+      <c r="R9" s="165"/>
+      <c r="S9" s="165"/>
+      <c r="T9" s="121"/>
+      <c r="U9" s="121"/>
+      <c r="V9" s="121"/>
+      <c r="W9" s="121"/>
+      <c r="X9" s="121"/>
+      <c r="Y9" s="121"/>
+      <c r="Z9" s="121"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="116">
+      <c r="C10" s="80">
         <v>1201</v>
       </c>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="117">
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="81">
         <v>1202</v>
       </c>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="116">
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="80">
         <v>1204</v>
       </c>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="118"/>
-      <c r="U10" s="117">
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="81">
         <v>1203</v>
       </c>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="118"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="82"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B11" s="138"/>
-      <c r="C11" s="134" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="135" t="s">
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="135"/>
-      <c r="K11" s="135"/>
-      <c r="L11" s="135"/>
-      <c r="M11" s="135"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="134" t="s">
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="P11" s="135"/>
-      <c r="Q11" s="135"/>
-      <c r="R11" s="135"/>
-      <c r="S11" s="135"/>
-      <c r="T11" s="136"/>
-      <c r="U11" s="135" t="s">
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="V11" s="135"/>
-      <c r="W11" s="135"/>
-      <c r="X11" s="135"/>
-      <c r="Y11" s="135"/>
-      <c r="Z11" s="136"/>
+      <c r="V11" s="75"/>
+      <c r="W11" s="75"/>
+      <c r="X11" s="75"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="76"/>
     </row>
     <row r="12" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="139"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="109" t="s">
+      <c r="E12" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="111"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="109" t="s">
+      <c r="K12" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-      <c r="N12" s="110"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
       <c r="O12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="P12" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="109" t="s">
+      <c r="Q12" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="111"/>
+      <c r="R12" s="84"/>
+      <c r="S12" s="84"/>
+      <c r="T12" s="85"/>
       <c r="U12" s="63" t="s">
         <v>11</v>
       </c>
       <c r="V12" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="W12" s="109" t="s">
+      <c r="W12" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="X12" s="110"/>
-      <c r="Y12" s="110"/>
-      <c r="Z12" s="111"/>
+      <c r="X12" s="84"/>
+      <c r="Y12" s="84"/>
+      <c r="Z12" s="85"/>
     </row>
     <row r="13" spans="2:26" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="55"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="19" t="s">
         <v>31</v>
       </c>
@@ -3620,7 +3657,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="21"/>
       <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="L13" s="70"/>
       <c r="M13" s="23" t="s">
         <v>31</v>
       </c>
@@ -3628,7 +3665,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
+      <c r="R13" s="64"/>
       <c r="S13" s="19" t="s">
         <v>31</v>
       </c>
@@ -3636,7 +3673,7 @@
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
       <c r="W13" s="18"/>
-      <c r="X13" s="26"/>
+      <c r="X13" s="64"/>
       <c r="Y13" s="19" t="s">
         <v>31</v>
       </c>
@@ -3647,7 +3684,7 @@
       <c r="C14" s="27"/>
       <c r="D14" s="28"/>
       <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="F14" s="72"/>
       <c r="G14" s="30" t="s">
         <v>31</v>
       </c>
@@ -3655,7 +3692,7 @@
       <c r="I14" s="32"/>
       <c r="J14" s="17"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="71"/>
       <c r="M14" s="19" t="s">
         <v>31</v>
       </c>
@@ -3663,7 +3700,7 @@
       <c r="O14" s="34"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
+      <c r="R14" s="68"/>
       <c r="S14" s="37" t="s">
         <v>31</v>
       </c>
@@ -3671,7 +3708,7 @@
       <c r="U14" s="28"/>
       <c r="V14" s="28"/>
       <c r="W14" s="29"/>
-      <c r="X14" s="39"/>
+      <c r="X14" s="65"/>
       <c r="Y14" s="30" t="s">
         <v>31</v>
       </c>
@@ -3682,7 +3719,7 @@
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="F15" s="72"/>
       <c r="G15" s="30" t="s">
         <v>31</v>
       </c>
@@ -3690,7 +3727,7 @@
       <c r="I15" s="40"/>
       <c r="J15" s="28"/>
       <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="L15" s="72"/>
       <c r="M15" s="30" t="s">
         <v>31</v>
       </c>
@@ -3698,7 +3735,7 @@
       <c r="O15" s="42"/>
       <c r="P15" s="43"/>
       <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
+      <c r="R15" s="69"/>
       <c r="S15" s="37" t="s">
         <v>31</v>
       </c>
@@ -3706,7 +3743,7 @@
       <c r="U15" s="28"/>
       <c r="V15" s="28"/>
       <c r="W15" s="29"/>
-      <c r="X15" s="39"/>
+      <c r="X15" s="65"/>
       <c r="Y15" s="30" t="s">
         <v>31</v>
       </c>
@@ -3717,7 +3754,7 @@
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="F16" s="72"/>
       <c r="G16" s="30" t="s">
         <v>31</v>
       </c>
@@ -3725,7 +3762,7 @@
       <c r="I16" s="40"/>
       <c r="J16" s="28"/>
       <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
+      <c r="L16" s="72"/>
       <c r="M16" s="30" t="s">
         <v>31</v>
       </c>
@@ -3733,7 +3770,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
+      <c r="R16" s="64"/>
       <c r="S16" s="19" t="s">
         <v>31</v>
       </c>
@@ -3741,7 +3778,7 @@
       <c r="U16" s="28"/>
       <c r="V16" s="28"/>
       <c r="W16" s="29"/>
-      <c r="X16" s="39"/>
+      <c r="X16" s="65"/>
       <c r="Y16" s="30" t="s">
         <v>31</v>
       </c>
@@ -3752,7 +3789,7 @@
       <c r="C17" s="46"/>
       <c r="D17" s="28"/>
       <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
+      <c r="F17" s="72"/>
       <c r="G17" s="30" t="s">
         <v>31</v>
       </c>
@@ -3760,7 +3797,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="28"/>
       <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
+      <c r="L17" s="72"/>
       <c r="M17" s="30" t="s">
         <v>31</v>
       </c>
@@ -3768,7 +3805,7 @@
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
       <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
+      <c r="R17" s="65"/>
       <c r="S17" s="30" t="s">
         <v>31</v>
       </c>
@@ -3776,7 +3813,7 @@
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
       <c r="W17" s="29"/>
-      <c r="X17" s="39"/>
+      <c r="X17" s="65"/>
       <c r="Y17" s="30" t="s">
         <v>31</v>
       </c>
@@ -3787,7 +3824,7 @@
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="F18" s="72"/>
       <c r="G18" s="30" t="s">
         <v>31</v>
       </c>
@@ -3795,7 +3832,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="28"/>
       <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="L18" s="72"/>
       <c r="M18" s="30" t="s">
         <v>31</v>
       </c>
@@ -3803,7 +3840,7 @@
       <c r="O18" s="27"/>
       <c r="P18" s="28"/>
       <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
+      <c r="R18" s="65"/>
       <c r="S18" s="30" t="s">
         <v>31</v>
       </c>
@@ -3811,7 +3848,7 @@
       <c r="U18" s="28"/>
       <c r="V18" s="28"/>
       <c r="W18" s="29"/>
-      <c r="X18" s="39"/>
+      <c r="X18" s="65"/>
       <c r="Y18" s="30" t="s">
         <v>31</v>
       </c>
@@ -3822,7 +3859,7 @@
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="30" t="s">
         <v>31</v>
       </c>
@@ -3830,7 +3867,7 @@
       <c r="I19" s="40"/>
       <c r="J19" s="28"/>
       <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
+      <c r="L19" s="72"/>
       <c r="M19" s="30" t="s">
         <v>31</v>
       </c>
@@ -3838,7 +3875,7 @@
       <c r="O19" s="27"/>
       <c r="P19" s="28"/>
       <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
+      <c r="R19" s="65"/>
       <c r="S19" s="30" t="s">
         <v>31</v>
       </c>
@@ -3846,7 +3883,7 @@
       <c r="U19" s="28"/>
       <c r="V19" s="28"/>
       <c r="W19" s="29"/>
-      <c r="X19" s="39"/>
+      <c r="X19" s="65"/>
       <c r="Y19" s="30" t="s">
         <v>31</v>
       </c>
@@ -3857,7 +3894,7 @@
       <c r="C20" s="34"/>
       <c r="D20" s="28"/>
       <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="F20" s="72"/>
       <c r="G20" s="30" t="s">
         <v>31</v>
       </c>
@@ -3865,7 +3902,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="28"/>
       <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="L20" s="72"/>
       <c r="M20" s="30" t="s">
         <v>31</v>
       </c>
@@ -3873,7 +3910,7 @@
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
       <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
+      <c r="R20" s="65"/>
       <c r="S20" s="30" t="s">
         <v>31</v>
       </c>
@@ -3881,7 +3918,7 @@
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
       <c r="W20" s="29"/>
-      <c r="X20" s="39"/>
+      <c r="X20" s="65"/>
       <c r="Y20" s="30" t="s">
         <v>31</v>
       </c>
@@ -3892,7 +3929,7 @@
       <c r="C21" s="27"/>
       <c r="D21" s="28"/>
       <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="30" t="s">
         <v>31</v>
       </c>
@@ -3900,7 +3937,7 @@
       <c r="I21" s="40"/>
       <c r="J21" s="28"/>
       <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="L21" s="72"/>
       <c r="M21" s="30" t="s">
         <v>31</v>
       </c>
@@ -3908,7 +3945,7 @@
       <c r="O21" s="27"/>
       <c r="P21" s="28"/>
       <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
+      <c r="R21" s="65"/>
       <c r="S21" s="30" t="s">
         <v>31</v>
       </c>
@@ -3916,7 +3953,7 @@
       <c r="U21" s="28"/>
       <c r="V21" s="28"/>
       <c r="W21" s="29"/>
-      <c r="X21" s="39"/>
+      <c r="X21" s="65"/>
       <c r="Y21" s="30" t="s">
         <v>31</v>
       </c>
@@ -3927,7 +3964,7 @@
       <c r="C22" s="27"/>
       <c r="D22" s="28"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="30" t="s">
         <v>31</v>
       </c>
@@ -3935,7 +3972,7 @@
       <c r="I22" s="40"/>
       <c r="J22" s="28"/>
       <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="L22" s="72"/>
       <c r="M22" s="30" t="s">
         <v>31</v>
       </c>
@@ -3943,7 +3980,7 @@
       <c r="O22" s="27"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
+      <c r="R22" s="65"/>
       <c r="S22" s="30" t="s">
         <v>31</v>
       </c>
@@ -3951,7 +3988,7 @@
       <c r="U22" s="28"/>
       <c r="V22" s="28"/>
       <c r="W22" s="29"/>
-      <c r="X22" s="39"/>
+      <c r="X22" s="65"/>
       <c r="Y22" s="30" t="s">
         <v>31</v>
       </c>
@@ -3962,7 +3999,7 @@
       <c r="C23" s="27"/>
       <c r="D23" s="28"/>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="F23" s="72"/>
       <c r="G23" s="30" t="s">
         <v>31</v>
       </c>
@@ -3970,7 +4007,7 @@
       <c r="I23" s="40"/>
       <c r="J23" s="28"/>
       <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="L23" s="72"/>
       <c r="M23" s="30" t="s">
         <v>31</v>
       </c>
@@ -3978,7 +4015,7 @@
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
       <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
+      <c r="R23" s="65"/>
       <c r="S23" s="30" t="s">
         <v>31</v>
       </c>
@@ -3986,7 +4023,7 @@
       <c r="U23" s="28"/>
       <c r="V23" s="28"/>
       <c r="W23" s="29"/>
-      <c r="X23" s="39"/>
+      <c r="X23" s="65"/>
       <c r="Y23" s="30" t="s">
         <v>31</v>
       </c>
@@ -3997,7 +4034,7 @@
       <c r="C24" s="27"/>
       <c r="D24" s="28"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="F24" s="72"/>
       <c r="G24" s="30" t="s">
         <v>31</v>
       </c>
@@ -4005,7 +4042,7 @@
       <c r="I24" s="40"/>
       <c r="J24" s="28"/>
       <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="L24" s="72"/>
       <c r="M24" s="30" t="s">
         <v>31</v>
       </c>
@@ -4013,7 +4050,7 @@
       <c r="O24" s="27"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
+      <c r="R24" s="65"/>
       <c r="S24" s="30" t="s">
         <v>31</v>
       </c>
@@ -4021,7 +4058,7 @@
       <c r="U24" s="28"/>
       <c r="V24" s="28"/>
       <c r="W24" s="29"/>
-      <c r="X24" s="39"/>
+      <c r="X24" s="65"/>
       <c r="Y24" s="30" t="s">
         <v>31</v>
       </c>
@@ -4032,7 +4069,7 @@
       <c r="C25" s="27"/>
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="30" t="s">
         <v>31</v>
       </c>
@@ -4040,7 +4077,7 @@
       <c r="I25" s="40"/>
       <c r="J25" s="28"/>
       <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="L25" s="72"/>
       <c r="M25" s="30" t="s">
         <v>31</v>
       </c>
@@ -4048,7 +4085,7 @@
       <c r="O25" s="27"/>
       <c r="P25" s="28"/>
       <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
+      <c r="R25" s="65"/>
       <c r="S25" s="30" t="s">
         <v>31</v>
       </c>
@@ -4056,7 +4093,7 @@
       <c r="U25" s="28"/>
       <c r="V25" s="28"/>
       <c r="W25" s="29"/>
-      <c r="X25" s="39"/>
+      <c r="X25" s="65"/>
       <c r="Y25" s="30" t="s">
         <v>31</v>
       </c>
@@ -4067,7 +4104,7 @@
       <c r="C26" s="27"/>
       <c r="D26" s="28"/>
       <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="F26" s="72"/>
       <c r="G26" s="30" t="s">
         <v>31</v>
       </c>
@@ -4075,7 +4112,7 @@
       <c r="I26" s="40"/>
       <c r="J26" s="28"/>
       <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="L26" s="72"/>
       <c r="M26" s="30" t="s">
         <v>31</v>
       </c>
@@ -4083,7 +4120,7 @@
       <c r="O26" s="27"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
+      <c r="R26" s="65"/>
       <c r="S26" s="30" t="s">
         <v>31</v>
       </c>
@@ -4091,7 +4128,7 @@
       <c r="U26" s="28"/>
       <c r="V26" s="28"/>
       <c r="W26" s="29"/>
-      <c r="X26" s="39"/>
+      <c r="X26" s="65"/>
       <c r="Y26" s="30" t="s">
         <v>31</v>
       </c>
@@ -4102,7 +4139,7 @@
       <c r="C27" s="27"/>
       <c r="D27" s="28"/>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="F27" s="72"/>
       <c r="G27" s="30" t="s">
         <v>31</v>
       </c>
@@ -4110,7 +4147,7 @@
       <c r="I27" s="40"/>
       <c r="J27" s="28"/>
       <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
+      <c r="L27" s="72"/>
       <c r="M27" s="30" t="s">
         <v>31</v>
       </c>
@@ -4118,7 +4155,7 @@
       <c r="O27" s="27"/>
       <c r="P27" s="28"/>
       <c r="Q27" s="39"/>
-      <c r="R27" s="39"/>
+      <c r="R27" s="65"/>
       <c r="S27" s="30" t="s">
         <v>31</v>
       </c>
@@ -4126,7 +4163,7 @@
       <c r="U27" s="28"/>
       <c r="V27" s="28"/>
       <c r="W27" s="29"/>
-      <c r="X27" s="39"/>
+      <c r="X27" s="65"/>
       <c r="Y27" s="30" t="s">
         <v>31</v>
       </c>
@@ -4143,7 +4180,7 @@
         <v>32</v>
       </c>
       <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="72"/>
       <c r="G28" s="30" t="s">
         <v>31</v>
       </c>
@@ -4151,7 +4188,7 @@
       <c r="I28" s="40"/>
       <c r="J28" s="28"/>
       <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
+      <c r="L28" s="72"/>
       <c r="M28" s="30" t="s">
         <v>31</v>
       </c>
@@ -4159,7 +4196,7 @@
       <c r="O28" s="27"/>
       <c r="P28" s="28"/>
       <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
+      <c r="R28" s="65"/>
       <c r="S28" s="30" t="s">
         <v>31</v>
       </c>
@@ -4167,7 +4204,7 @@
       <c r="U28" s="28"/>
       <c r="V28" s="28"/>
       <c r="W28" s="29"/>
-      <c r="X28" s="39"/>
+      <c r="X28" s="65"/>
       <c r="Y28" s="30" t="s">
         <v>31</v>
       </c>
@@ -4178,7 +4215,7 @@
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
       <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="30" t="s">
         <v>31</v>
       </c>
@@ -4186,7 +4223,7 @@
       <c r="I29" s="40"/>
       <c r="J29" s="28"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
+      <c r="L29" s="72"/>
       <c r="M29" s="30" t="s">
         <v>31</v>
       </c>
@@ -4194,7 +4231,7 @@
       <c r="O29" s="27"/>
       <c r="P29" s="28"/>
       <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
+      <c r="R29" s="65"/>
       <c r="S29" s="30" t="s">
         <v>31</v>
       </c>
@@ -4202,7 +4239,7 @@
       <c r="U29" s="28"/>
       <c r="V29" s="28"/>
       <c r="W29" s="29"/>
-      <c r="X29" s="39"/>
+      <c r="X29" s="65"/>
       <c r="Y29" s="30" t="s">
         <v>31</v>
       </c>
@@ -4213,7 +4250,7 @@
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
       <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="30" t="s">
         <v>31</v>
       </c>
@@ -4221,7 +4258,7 @@
       <c r="I30" s="40"/>
       <c r="J30" s="28"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
+      <c r="L30" s="72"/>
       <c r="M30" s="30" t="s">
         <v>31</v>
       </c>
@@ -4229,7 +4266,7 @@
       <c r="O30" s="27"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
+      <c r="R30" s="65"/>
       <c r="S30" s="30" t="s">
         <v>31</v>
       </c>
@@ -4237,7 +4274,7 @@
       <c r="U30" s="28"/>
       <c r="V30" s="28"/>
       <c r="W30" s="29"/>
-      <c r="X30" s="39"/>
+      <c r="X30" s="65"/>
       <c r="Y30" s="30" t="s">
         <v>31</v>
       </c>
@@ -4248,7 +4285,7 @@
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="F31" s="72"/>
       <c r="G31" s="30" t="s">
         <v>31</v>
       </c>
@@ -4256,7 +4293,7 @@
       <c r="I31" s="40"/>
       <c r="J31" s="28"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
+      <c r="L31" s="72"/>
       <c r="M31" s="30" t="s">
         <v>31</v>
       </c>
@@ -4264,7 +4301,7 @@
       <c r="O31" s="27"/>
       <c r="P31" s="28"/>
       <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
+      <c r="R31" s="65"/>
       <c r="S31" s="30" t="s">
         <v>31</v>
       </c>
@@ -4272,7 +4309,7 @@
       <c r="U31" s="28"/>
       <c r="V31" s="28"/>
       <c r="W31" s="29"/>
-      <c r="X31" s="39"/>
+      <c r="X31" s="65"/>
       <c r="Y31" s="30" t="s">
         <v>31</v>
       </c>
@@ -4283,7 +4320,7 @@
       <c r="C32" s="27"/>
       <c r="D32" s="28"/>
       <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
+      <c r="F32" s="72"/>
       <c r="G32" s="30" t="s">
         <v>31</v>
       </c>
@@ -4291,7 +4328,7 @@
       <c r="I32" s="40"/>
       <c r="J32" s="28"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
+      <c r="L32" s="72"/>
       <c r="M32" s="30" t="s">
         <v>31</v>
       </c>
@@ -4299,7 +4336,7 @@
       <c r="O32" s="27"/>
       <c r="P32" s="28"/>
       <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
+      <c r="R32" s="65"/>
       <c r="S32" s="30" t="s">
         <v>31</v>
       </c>
@@ -4307,7 +4344,7 @@
       <c r="U32" s="28"/>
       <c r="V32" s="28"/>
       <c r="W32" s="29"/>
-      <c r="X32" s="39"/>
+      <c r="X32" s="65"/>
       <c r="Y32" s="30" t="s">
         <v>31</v>
       </c>
@@ -4318,7 +4355,7 @@
       <c r="C33" s="27"/>
       <c r="D33" s="28"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="F33" s="72"/>
       <c r="G33" s="30" t="s">
         <v>31</v>
       </c>
@@ -4326,7 +4363,7 @@
       <c r="I33" s="40"/>
       <c r="J33" s="28"/>
       <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
+      <c r="L33" s="72"/>
       <c r="M33" s="30" t="s">
         <v>31</v>
       </c>
@@ -4334,7 +4371,7 @@
       <c r="O33" s="27"/>
       <c r="P33" s="28"/>
       <c r="Q33" s="39"/>
-      <c r="R33" s="39"/>
+      <c r="R33" s="65"/>
       <c r="S33" s="30" t="s">
         <v>31</v>
       </c>
@@ -4342,7 +4379,7 @@
       <c r="U33" s="28"/>
       <c r="V33" s="28"/>
       <c r="W33" s="29"/>
-      <c r="X33" s="39"/>
+      <c r="X33" s="65"/>
       <c r="Y33" s="30" t="s">
         <v>31</v>
       </c>
@@ -4353,7 +4390,7 @@
       <c r="C34" s="27"/>
       <c r="D34" s="28"/>
       <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="F34" s="72"/>
       <c r="G34" s="30" t="s">
         <v>31</v>
       </c>
@@ -4361,7 +4398,7 @@
       <c r="I34" s="40"/>
       <c r="J34" s="28"/>
       <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
+      <c r="L34" s="72"/>
       <c r="M34" s="30" t="s">
         <v>31</v>
       </c>
@@ -4369,7 +4406,7 @@
       <c r="O34" s="27"/>
       <c r="P34" s="28"/>
       <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
+      <c r="R34" s="65"/>
       <c r="S34" s="30" t="s">
         <v>31</v>
       </c>
@@ -4377,7 +4414,7 @@
       <c r="U34" s="28"/>
       <c r="V34" s="28"/>
       <c r="W34" s="29"/>
-      <c r="X34" s="39"/>
+      <c r="X34" s="65"/>
       <c r="Y34" s="30" t="s">
         <v>31</v>
       </c>
@@ -4388,7 +4425,7 @@
       <c r="C35" s="27"/>
       <c r="D35" s="28"/>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="F35" s="72"/>
       <c r="G35" s="30" t="s">
         <v>31</v>
       </c>
@@ -4396,7 +4433,7 @@
       <c r="I35" s="40"/>
       <c r="J35" s="28"/>
       <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
+      <c r="L35" s="72"/>
       <c r="M35" s="30" t="s">
         <v>31</v>
       </c>
@@ -4404,7 +4441,7 @@
       <c r="O35" s="27"/>
       <c r="P35" s="28"/>
       <c r="Q35" s="39"/>
-      <c r="R35" s="39"/>
+      <c r="R35" s="65"/>
       <c r="S35" s="30" t="s">
         <v>31</v>
       </c>
@@ -4412,7 +4449,7 @@
       <c r="U35" s="28"/>
       <c r="V35" s="28"/>
       <c r="W35" s="29"/>
-      <c r="X35" s="39"/>
+      <c r="X35" s="65"/>
       <c r="Y35" s="30" t="s">
         <v>31</v>
       </c>
@@ -4423,7 +4460,7 @@
       <c r="C36" s="47"/>
       <c r="D36" s="48"/>
       <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="F36" s="73"/>
       <c r="G36" s="50" t="s">
         <v>31</v>
       </c>
@@ -4431,7 +4468,7 @@
       <c r="I36" s="52"/>
       <c r="J36" s="48"/>
       <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
+      <c r="L36" s="73"/>
       <c r="M36" s="50" t="s">
         <v>31</v>
       </c>
@@ -4439,7 +4476,7 @@
       <c r="O36" s="47"/>
       <c r="P36" s="48"/>
       <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
+      <c r="R36" s="66"/>
       <c r="S36" s="50" t="s">
         <v>31</v>
       </c>
@@ -4447,7 +4484,7 @@
       <c r="U36" s="48"/>
       <c r="V36" s="48"/>
       <c r="W36" s="49"/>
-      <c r="X36" s="53"/>
+      <c r="X36" s="66"/>
       <c r="Y36" s="50" t="s">
         <v>31</v>
       </c>
@@ -4455,328 +4492,313 @@
     </row>
     <row r="37" spans="2:26" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="59"/>
-      <c r="C37" s="112" t="s">
+      <c r="C37" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="113"/>
+      <c r="D37" s="118"/>
       <c r="E37" s="60"/>
-      <c r="F37" s="60">
-        <f>SUM(F13:F36)</f>
-        <v>0</v>
-      </c>
+      <c r="F37" s="67"/>
       <c r="G37" s="61" t="s">
         <v>31</v>
       </c>
       <c r="H37" s="60"/>
-      <c r="I37" s="112" t="s">
+      <c r="I37" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="114">
+      <c r="J37" s="119">
         <v>20</v>
       </c>
       <c r="K37" s="60"/>
-      <c r="L37" s="60">
-        <f>SUM(L13:L36)</f>
-        <v>0</v>
-      </c>
+      <c r="L37" s="67"/>
       <c r="M37" s="61" t="s">
         <v>31</v>
       </c>
       <c r="N37" s="60"/>
-      <c r="O37" s="112" t="s">
+      <c r="O37" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="P37" s="114">
+      <c r="P37" s="119">
         <v>20</v>
       </c>
       <c r="Q37" s="60"/>
-      <c r="R37" s="60">
-        <f>SUM(R13:R36)</f>
-        <v>0</v>
-      </c>
+      <c r="R37" s="67"/>
       <c r="S37" s="50" t="s">
         <v>31</v>
       </c>
       <c r="T37" s="60"/>
-      <c r="U37" s="112" t="s">
+      <c r="U37" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="V37" s="115"/>
+      <c r="V37" s="120"/>
       <c r="W37" s="60"/>
-      <c r="X37" s="60">
-        <f>SUM(X13:X36)</f>
-        <v>0</v>
-      </c>
+      <c r="X37" s="67"/>
       <c r="Y37" s="61" t="s">
         <v>31</v>
       </c>
       <c r="Z37" s="62"/>
     </row>
     <row r="38" spans="2:26" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
-      <c r="P38" s="101"/>
-      <c r="Q38" s="101"/>
-      <c r="R38" s="101"/>
-      <c r="S38" s="101"/>
-      <c r="T38" s="101"/>
-      <c r="U38" s="101"/>
-      <c r="V38" s="101"/>
-      <c r="W38" s="101"/>
-      <c r="X38" s="101"/>
-      <c r="Y38" s="101"/>
-      <c r="Z38" s="102"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="109"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="109"/>
+      <c r="P38" s="109"/>
+      <c r="Q38" s="109"/>
+      <c r="R38" s="109"/>
+      <c r="S38" s="109"/>
+      <c r="T38" s="109"/>
+      <c r="U38" s="109"/>
+      <c r="V38" s="109"/>
+      <c r="W38" s="109"/>
+      <c r="X38" s="109"/>
+      <c r="Y38" s="109"/>
+      <c r="Z38" s="110"/>
     </row>
     <row r="39" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="104"/>
-      <c r="D39" s="104"/>
-      <c r="E39" s="104"/>
-      <c r="F39" s="104"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="104"/>
-      <c r="I39" s="104"/>
-      <c r="J39" s="104"/>
-      <c r="K39" s="104"/>
-      <c r="L39" s="104"/>
-      <c r="M39" s="104"/>
-      <c r="N39" s="104"/>
-      <c r="O39" s="104"/>
-      <c r="P39" s="104"/>
-      <c r="Q39" s="104"/>
-      <c r="R39" s="104"/>
-      <c r="S39" s="104"/>
-      <c r="T39" s="104"/>
-      <c r="U39" s="104"/>
-      <c r="V39" s="104"/>
-      <c r="W39" s="104"/>
-      <c r="X39" s="104"/>
-      <c r="Y39" s="104"/>
-      <c r="Z39" s="105"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="112"/>
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="112"/>
+      <c r="M39" s="112"/>
+      <c r="N39" s="112"/>
+      <c r="O39" s="112"/>
+      <c r="P39" s="112"/>
+      <c r="Q39" s="112"/>
+      <c r="R39" s="112"/>
+      <c r="S39" s="112"/>
+      <c r="T39" s="112"/>
+      <c r="U39" s="112"/>
+      <c r="V39" s="112"/>
+      <c r="W39" s="112"/>
+      <c r="X39" s="112"/>
+      <c r="Y39" s="112"/>
+      <c r="Z39" s="113"/>
     </row>
     <row r="40" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="106"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="107"/>
-      <c r="N40" s="107"/>
-      <c r="O40" s="107"/>
-      <c r="P40" s="107"/>
-      <c r="Q40" s="107"/>
-      <c r="R40" s="107"/>
-      <c r="S40" s="107"/>
-      <c r="T40" s="107"/>
-      <c r="U40" s="107"/>
-      <c r="V40" s="107"/>
-      <c r="W40" s="107"/>
-      <c r="X40" s="107"/>
-      <c r="Y40" s="107"/>
-      <c r="Z40" s="108"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="115"/>
+      <c r="H40" s="115"/>
+      <c r="I40" s="115"/>
+      <c r="J40" s="115"/>
+      <c r="K40" s="115"/>
+      <c r="L40" s="115"/>
+      <c r="M40" s="115"/>
+      <c r="N40" s="115"/>
+      <c r="O40" s="115"/>
+      <c r="P40" s="115"/>
+      <c r="Q40" s="115"/>
+      <c r="R40" s="115"/>
+      <c r="S40" s="115"/>
+      <c r="T40" s="115"/>
+      <c r="U40" s="115"/>
+      <c r="V40" s="115"/>
+      <c r="W40" s="115"/>
+      <c r="X40" s="115"/>
+      <c r="Y40" s="115"/>
+      <c r="Z40" s="116"/>
     </row>
     <row r="41" spans="2:26" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="125"/>
-      <c r="C41" s="126"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="126"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="126"/>
-      <c r="H41" s="126"/>
-      <c r="I41" s="126"/>
-      <c r="J41" s="126"/>
-      <c r="K41" s="126"/>
-      <c r="L41" s="126"/>
-      <c r="M41" s="126"/>
-      <c r="N41" s="126"/>
-      <c r="O41" s="126"/>
-      <c r="P41" s="126"/>
-      <c r="Q41" s="126"/>
-      <c r="R41" s="126"/>
-      <c r="S41" s="126"/>
-      <c r="T41" s="126"/>
-      <c r="U41" s="126"/>
-      <c r="V41" s="126"/>
-      <c r="W41" s="126"/>
-      <c r="X41" s="126"/>
-      <c r="Y41" s="126"/>
-      <c r="Z41" s="127"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="93"/>
+      <c r="P41" s="93"/>
+      <c r="Q41" s="93"/>
+      <c r="R41" s="93"/>
+      <c r="S41" s="93"/>
+      <c r="T41" s="93"/>
+      <c r="U41" s="93"/>
+      <c r="V41" s="93"/>
+      <c r="W41" s="93"/>
+      <c r="X41" s="93"/>
+      <c r="Y41" s="93"/>
+      <c r="Z41" s="94"/>
     </row>
     <row r="42" spans="2:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="128" t="s">
+      <c r="B42" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="129"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="129"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="129"/>
-      <c r="H42" s="129"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="131" t="s">
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="K42" s="132"/>
-      <c r="L42" s="132"/>
-      <c r="M42" s="132"/>
-      <c r="N42" s="132"/>
-      <c r="O42" s="132"/>
-      <c r="P42" s="132"/>
-      <c r="Q42" s="132"/>
-      <c r="R42" s="133"/>
-      <c r="S42" s="131" t="s">
+      <c r="K42" s="99"/>
+      <c r="L42" s="99"/>
+      <c r="M42" s="99"/>
+      <c r="N42" s="99"/>
+      <c r="O42" s="99"/>
+      <c r="P42" s="99"/>
+      <c r="Q42" s="99"/>
+      <c r="R42" s="100"/>
+      <c r="S42" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="T42" s="132"/>
-      <c r="U42" s="132"/>
-      <c r="V42" s="132"/>
-      <c r="W42" s="132"/>
-      <c r="X42" s="132"/>
-      <c r="Y42" s="132"/>
-      <c r="Z42" s="133"/>
+      <c r="T42" s="99"/>
+      <c r="U42" s="99"/>
+      <c r="V42" s="99"/>
+      <c r="W42" s="99"/>
+      <c r="X42" s="99"/>
+      <c r="Y42" s="99"/>
+      <c r="Z42" s="100"/>
     </row>
     <row r="43" spans="2:26" s="54" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="97" t="s">
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
-      <c r="Q43" s="98"/>
-      <c r="R43" s="99"/>
-      <c r="S43" s="97" t="s">
+      <c r="K43" s="105"/>
+      <c r="L43" s="105"/>
+      <c r="M43" s="105"/>
+      <c r="N43" s="105"/>
+      <c r="O43" s="105"/>
+      <c r="P43" s="105"/>
+      <c r="Q43" s="105"/>
+      <c r="R43" s="106"/>
+      <c r="S43" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="T43" s="98"/>
-      <c r="U43" s="98"/>
-      <c r="V43" s="98"/>
-      <c r="W43" s="98"/>
-      <c r="X43" s="98"/>
-      <c r="Y43" s="98"/>
-      <c r="Z43" s="99"/>
+      <c r="T43" s="105"/>
+      <c r="U43" s="105"/>
+      <c r="V43" s="105"/>
+      <c r="W43" s="105"/>
+      <c r="X43" s="105"/>
+      <c r="Y43" s="105"/>
+      <c r="Z43" s="106"/>
     </row>
     <row r="44" spans="2:26" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="94" t="s">
+      <c r="B44" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="97" t="s">
+      <c r="C44" s="102"/>
+      <c r="D44" s="102"/>
+      <c r="E44" s="102"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="102"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="K44" s="98"/>
-      <c r="L44" s="98"/>
-      <c r="M44" s="98"/>
-      <c r="N44" s="98"/>
-      <c r="O44" s="98"/>
-      <c r="P44" s="98"/>
-      <c r="Q44" s="98"/>
-      <c r="R44" s="99"/>
-      <c r="S44" s="97" t="s">
+      <c r="K44" s="105"/>
+      <c r="L44" s="105"/>
+      <c r="M44" s="105"/>
+      <c r="N44" s="105"/>
+      <c r="O44" s="105"/>
+      <c r="P44" s="105"/>
+      <c r="Q44" s="105"/>
+      <c r="R44" s="106"/>
+      <c r="S44" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="T44" s="98"/>
-      <c r="U44" s="98"/>
-      <c r="V44" s="98"/>
-      <c r="W44" s="98"/>
-      <c r="X44" s="98"/>
-      <c r="Y44" s="98"/>
-      <c r="Z44" s="99"/>
+      <c r="T44" s="105"/>
+      <c r="U44" s="105"/>
+      <c r="V44" s="105"/>
+      <c r="W44" s="105"/>
+      <c r="X44" s="105"/>
+      <c r="Y44" s="105"/>
+      <c r="Z44" s="106"/>
     </row>
     <row r="45" spans="2:26" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="119" t="s">
+      <c r="B45" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="121"/>
-      <c r="J45" s="122" t="s">
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="K45" s="123"/>
-      <c r="L45" s="123"/>
-      <c r="M45" s="123"/>
-      <c r="N45" s="123"/>
-      <c r="O45" s="123"/>
-      <c r="P45" s="123"/>
-      <c r="Q45" s="123"/>
-      <c r="R45" s="124"/>
-      <c r="S45" s="122" t="s">
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
+      <c r="M45" s="90"/>
+      <c r="N45" s="90"/>
+      <c r="O45" s="90"/>
+      <c r="P45" s="90"/>
+      <c r="Q45" s="90"/>
+      <c r="R45" s="91"/>
+      <c r="S45" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="T45" s="123"/>
-      <c r="U45" s="123"/>
-      <c r="V45" s="123"/>
-      <c r="W45" s="123"/>
-      <c r="X45" s="123"/>
-      <c r="Y45" s="123"/>
-      <c r="Z45" s="124"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
+      <c r="X45" s="90"/>
+      <c r="Y45" s="90"/>
+      <c r="Z45" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="O11:T11"/>
-    <mergeCell ref="U11:Z11"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="J45:R45"/>
-    <mergeCell ref="S45:Z45"/>
-    <mergeCell ref="B41:Z41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="J42:R42"/>
-    <mergeCell ref="S42:Z42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="J43:R43"/>
-    <mergeCell ref="S43:Z43"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G9:N9"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="T9:Z9"/>
+    <mergeCell ref="B2:Z3"/>
+    <mergeCell ref="Q6:Z6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="B4:W5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:Z7"/>
+    <mergeCell ref="T8:Z8"/>
+    <mergeCell ref="O8:S8"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:N8"/>
     <mergeCell ref="B44:I44"/>
@@ -4793,22 +4815,25 @@
     <mergeCell ref="U37:V37"/>
     <mergeCell ref="O10:T10"/>
     <mergeCell ref="U10:Z10"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="G9:N9"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="T9:Z9"/>
-    <mergeCell ref="B2:Z3"/>
-    <mergeCell ref="Q6:Z6"/>
-    <mergeCell ref="J6:P6"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="B4:W5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:Z7"/>
-    <mergeCell ref="T8:Z8"/>
-    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="J45:R45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="B41:Z41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="J42:R42"/>
+    <mergeCell ref="S42:Z42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="J43:R43"/>
+    <mergeCell ref="S43:Z43"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="O11:T11"/>
+    <mergeCell ref="U11:Z11"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="K12:N12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.98425196850393704" footer="0.31496062992125984"/>
@@ -4822,7 +4847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:Q29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29:G29"/>
     </sheetView>
   </sheetViews>
@@ -4840,16 +4865,16 @@
   <sheetData>
     <row r="1" spans="2:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -4857,16 +4882,16 @@
       <c r="P2" s="6"/>
     </row>
     <row r="3" spans="2:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
-      <c r="K3" s="150"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -4874,17 +4899,17 @@
       <c r="P3" s="6"/>
     </row>
     <row r="4" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
       <c r="K4" s="8" t="s">
         <v>64</v>
       </c>
@@ -4895,15 +4920,15 @@
       <c r="P4" s="6"/>
     </row>
     <row r="5" spans="2:17" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="140"/>
       <c r="K5" s="7" t="s">
         <v>62</v>
       </c>
@@ -4915,397 +4940,373 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
     </row>
     <row r="7" spans="2:17" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="154" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="152"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
-      <c r="K7" s="152"/>
+      <c r="C7" s="154"/>
+      <c r="D7" s="154"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="154"/>
+      <c r="G7" s="154"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
+      <c r="K7" s="154"/>
     </row>
     <row r="8" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
+      <c r="C8" s="150"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="150"/>
+      <c r="F8" s="150"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="150"/>
+      <c r="K8" s="150"/>
     </row>
     <row r="9" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="151" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
+      <c r="C9" s="151"/>
+      <c r="D9" s="151"/>
+      <c r="E9" s="151"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="151"/>
+      <c r="K9" s="151"/>
     </row>
     <row r="10" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="154"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="151"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="151"/>
+      <c r="K10" s="151"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="154" t="s">
+      <c r="B11" s="151" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="154"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="154"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="154"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="151"/>
+      <c r="K11" s="151"/>
     </row>
     <row r="12" spans="2:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="154" t="s">
+      <c r="B12" s="151" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="151"/>
+      <c r="K12" s="151"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="154" t="s">
+      <c r="B13" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="154"/>
-      <c r="D13" s="154"/>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="C13" s="151"/>
+      <c r="D13" s="151"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="151"/>
+      <c r="K13" s="151"/>
     </row>
     <row r="14" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="151" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="151"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="151"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="151"/>
     </row>
     <row r="15" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="153" t="s">
+      <c r="B15" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="150"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142" t="s">
+      <c r="D16" s="163"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
     </row>
     <row r="17" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="140" t="s">
+      <c r="C17" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="141"/>
-      <c r="K17" s="141"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="158"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="158"/>
     </row>
     <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="158"/>
+      <c r="J18" s="158"/>
+      <c r="K18" s="158"/>
     </row>
     <row r="19" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
     </row>
     <row r="20" spans="2:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="143" t="s">
+      <c r="C20" s="164" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="164"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158"/>
+      <c r="J20" s="158"/>
+      <c r="K20" s="158"/>
     </row>
     <row r="21" spans="2:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="140" t="s">
+      <c r="C21" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="141"/>
-      <c r="K21" s="141"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158"/>
+      <c r="J21" s="158"/>
+      <c r="K21" s="158"/>
     </row>
     <row r="22" spans="2:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="141"/>
+      <c r="D22" s="159"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="158"/>
+      <c r="K22" s="158"/>
     </row>
     <row r="23" spans="2:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="159" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="141"/>
-      <c r="K23" s="141"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158"/>
+      <c r="J23" s="158"/>
+      <c r="K23" s="158"/>
     </row>
     <row r="24" spans="2:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="159" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="141"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="158"/>
+      <c r="K24" s="158"/>
     </row>
     <row r="25" spans="2:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="141"/>
-      <c r="K25" s="141"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="158"/>
+      <c r="K25" s="158"/>
     </row>
     <row r="26" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="145"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="141"/>
-      <c r="J26" s="141"/>
-      <c r="K26" s="141"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="157"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="158"/>
     </row>
     <row r="27" spans="2:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="144" t="s">
+      <c r="C27" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="146"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="149"/>
+      <c r="D27" s="156"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="161"/>
+      <c r="J27" s="161"/>
+      <c r="K27" s="162"/>
     </row>
     <row r="28" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="144" t="s">
+      <c r="C28" s="155" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="148"/>
-      <c r="K28" s="149"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="157"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="161"/>
+      <c r="J28" s="161"/>
+      <c r="K28" s="162"/>
     </row>
     <row r="29" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="144" t="s">
+      <c r="C29" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="145"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="145"/>
-      <c r="G29" s="146"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="148"/>
-      <c r="K29" s="149"/>
+      <c r="D29" s="156"/>
+      <c r="E29" s="156"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="157"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="161"/>
+      <c r="J29" s="161"/>
+      <c r="K29" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B4:J5"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="H16:K16"/>
@@ -5322,6 +5323,30 @@
     <mergeCell ref="H22:K22"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="H18:K18"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" orientation="portrait" r:id="rId1"/>

</xml_diff>